<commit_message>
upgraded node-xlsx and used forked xlsx
</commit_message>
<xml_diff>
--- a/test/fixtures/test.xlsx
+++ b/test/fixtures/test.xlsx
@@ -1,40 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
-  </bookViews>
+  <workbookPr date1904="false"/>
   <sheets>
-    <sheet name="hello" sheetId="1" r:id="rId1"/>
+    <sheet name="mySheetName" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>B1</t>
-  </si>
-  <si>
-    <t>A2</t>
-  </si>
-  <si>
-    <t>B2</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -61,19 +39,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -123,10 +97,10 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="MS P????"/>
-        <a:font script="Hang" typeface="?? ??"/>
-        <a:font script="Hans" typeface="??"/>
-        <a:font script="Hant" typeface="????"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -158,10 +132,10 @@
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="MS P????"/>
-        <a:font script="Hang" typeface="?? ??"/>
-        <a:font script="Hans" typeface="??"/>
-        <a:font script="Hant" typeface="????"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -222,20 +196,16 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -357,36 +327,98 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
   <sheetData>
-    <row r="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" t="b">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="D2" t="str">
+        <v>sheetjs</v>
       </c>
     </row>
-    <row r="2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>foo</v>
+      </c>
+      <c r="B3" t="str">
+        <v>bar</v>
+      </c>
+      <c r="C3" s="1">
+        <v>41689.604166666664</v>
+      </c>
+      <c r="D3" t="str">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>baz</v>
+      </c>
+      <c r="C4" t="str">
+        <v>qux</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>